<commit_message>
Modificacion sobre acciones correctivas Marzo
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Acciones_Correctivas-150331.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Acciones_Correctivas-150331.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Acciones correctivas</t>
   </si>
@@ -52,13 +52,16 @@
     <t>Fidel Reyna</t>
   </si>
   <si>
-    <t>Abierto</t>
-  </si>
-  <si>
-    <t>31/04/2015</t>
-  </si>
-  <si>
-    <t>Cerrado</t>
+    <t>Proceso</t>
+  </si>
+  <si>
+    <t>Generar lo mas pronto posible las encuestas de satisfaccion</t>
+  </si>
+  <si>
+    <t>Por omicion a la generacion de encuestas de satisfaccion existen resultados invalidos en la seccion de satisfaccion</t>
+  </si>
+  <si>
+    <t>Jovanny Zepeda</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -193,6 +196,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -518,7 +524,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -593,7 +599,7 @@
       <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -608,31 +614,29 @@
       <c r="H5" s="7">
         <v>42094</v>
       </c>
-      <c r="I5" s="7">
-        <v>42094</v>
-      </c>
+      <c r="I5" s="7"/>
       <c r="J5" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="120" x14ac:dyDescent="0.2">
       <c r="C6" s="11">
         <v>2</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F6" s="5">
-        <v>42062</v>
+        <v>42094</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H6" s="7">
+        <v>42124</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="8" t="s">

</xml_diff>